<commit_message>
adaugare fisiere baza de date
</commit_message>
<xml_diff>
--- a/website/Users.xlsx
+++ b/website/Users.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UltimaSansa\website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40754\Desktop\hackitall\UltimaSansa\website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3689E2-5FE6-4882-B801-87664F1480BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2CB7F2-B4EE-4F53-BE1A-E2E9AF3D643D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6731FC37-29E0-4F98-8863-FC5F1890B5EB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6731FC37-29E0-4F98-8863-FC5F1890B5EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
     <t>email</t>
   </si>
   <si>
-    <t>andreamargareta@gmail.com</t>
+    <t>oclock@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Temă Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -436,7 +436,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -457,7 +457,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>

</xml_diff>